<commit_message>
remove whitespace from node_fields.xlsx
</commit_message>
<xml_diff>
--- a/data/node_fields.xlsx
+++ b/data/node_fields.xlsx
@@ -8,17 +8,26 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\nyou045\git\melanoma\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{134CEFFC-2A7E-4E8A-A378-2FB27BEBC127}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8FE86B99-1E3E-46BC-A07F-07B56B55FFF8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
@@ -36,405 +45,126 @@
     <t>Other Node Fields</t>
   </si>
   <si>
-    <t>ro </t>
-  </si>
-  <si>
-    <t>right occipital </t>
-  </si>
-  <si>
-    <t>lo </t>
-  </si>
-  <si>
     <t>left occipital</t>
   </si>
   <si>
-    <t>rprea </t>
-  </si>
-  <si>
-    <t>right preauricular </t>
-  </si>
-  <si>
-    <t>lprea </t>
-  </si>
-  <si>
     <t>left preauricular</t>
   </si>
   <si>
-    <t>rc1 </t>
-  </si>
-  <si>
-    <t>right cervical level i </t>
-  </si>
-  <si>
-    <t>lc1 </t>
-  </si>
-  <si>
     <t>left cervical level i</t>
   </si>
   <si>
-    <t>rc2 </t>
-  </si>
-  <si>
-    <t>right cervical level ii </t>
-  </si>
-  <si>
-    <t>lc2 </t>
-  </si>
-  <si>
     <t>left cervical level ii</t>
   </si>
   <si>
-    <t>rc3 </t>
-  </si>
-  <si>
-    <t>right cervical level iii </t>
-  </si>
-  <si>
-    <t>lc3 </t>
-  </si>
-  <si>
     <t>left cervical level iii</t>
   </si>
   <si>
-    <t>rc4 </t>
-  </si>
-  <si>
-    <t>right cervical level iv </t>
-  </si>
-  <si>
-    <t>lc4 </t>
-  </si>
-  <si>
     <t>left cervical level iv</t>
   </si>
   <si>
-    <t>rc5 </t>
-  </si>
-  <si>
-    <t>right cervical level v </t>
-  </si>
-  <si>
-    <t>lc5 </t>
-  </si>
-  <si>
     <t>left cervical level v</t>
   </si>
   <si>
-    <t>rc6 </t>
-  </si>
-  <si>
-    <t>right cervical level vi </t>
-  </si>
-  <si>
-    <t>lc6 </t>
-  </si>
-  <si>
     <t>left cervical level vi</t>
   </si>
   <si>
-    <t>rc7 </t>
-  </si>
-  <si>
-    <t>right cervical level vii </t>
-  </si>
-  <si>
-    <t>lc7 </t>
-  </si>
-  <si>
     <t>left cervical level vii</t>
   </si>
   <si>
-    <t>rsc </t>
-  </si>
-  <si>
-    <t>right supraclavicular fossa </t>
-  </si>
-  <si>
-    <t>lsc </t>
-  </si>
-  <si>
     <t>left supraclavicular fossa</t>
   </si>
   <si>
-    <t>rsm </t>
-  </si>
-  <si>
-    <t>right submental </t>
-  </si>
-  <si>
-    <t>lsm </t>
-  </si>
-  <si>
     <t>left submental</t>
   </si>
   <si>
-    <t>sm </t>
-  </si>
-  <si>
     <t>submental</t>
   </si>
   <si>
-    <t>rbu </t>
-  </si>
-  <si>
-    <t>right buccal </t>
-  </si>
-  <si>
-    <t>lbu </t>
-  </si>
-  <si>
     <t>left buccal</t>
   </si>
   <si>
-    <t>raa </t>
-  </si>
-  <si>
     <t>right axilla anterior or antero/pectoral group (levels I,II,III)</t>
   </si>
   <si>
-    <t>laa </t>
-  </si>
-  <si>
     <t>left axilla anterior or antero/pectoral  group (levels I,II,III)</t>
   </si>
   <si>
-    <t>ram </t>
-  </si>
-  <si>
-    <t>right mid axilla (levels I,II,III) </t>
-  </si>
-  <si>
-    <t>lam </t>
-  </si>
-  <si>
     <t>left mid axilla (levels I,II,III)</t>
   </si>
   <si>
-    <t>rap </t>
-  </si>
-  <si>
-    <t>right posterior axilla (levels I,II,III) </t>
-  </si>
-  <si>
-    <t>lap </t>
-  </si>
-  <si>
     <t>left posterior axilla (levels I,II,III)</t>
   </si>
   <si>
-    <t>repit </t>
-  </si>
-  <si>
-    <t>right epitrochlear </t>
-  </si>
-  <si>
-    <t>lepit </t>
-  </si>
-  <si>
     <t>left epitrochlear</t>
   </si>
   <si>
-    <t>ric </t>
-  </si>
-  <si>
-    <t>right infraclavicular </t>
-  </si>
-  <si>
-    <t>lic </t>
-  </si>
-  <si>
     <t>left infraclavicular</t>
   </si>
   <si>
-    <t>rtis </t>
-  </si>
-  <si>
     <t>right right triangular intermuscular space (tis)</t>
   </si>
   <si>
-    <t>ltis </t>
-  </si>
-  <si>
     <t>left tis</t>
   </si>
   <si>
-    <t>rip </t>
-  </si>
-  <si>
-    <t>right interpectoral </t>
-  </si>
-  <si>
-    <t>lip </t>
-  </si>
-  <si>
     <t>left interpectoral</t>
   </si>
   <si>
-    <t>rim </t>
-  </si>
-  <si>
-    <t>right internal mammary </t>
-  </si>
-  <si>
-    <t>lim </t>
-  </si>
-  <si>
     <t>left internal mammary</t>
   </si>
   <si>
-    <t>rcm </t>
-  </si>
-  <si>
-    <t>right costal margin </t>
-  </si>
-  <si>
-    <t>lcm </t>
-  </si>
-  <si>
     <t>left costal margin</t>
   </si>
   <si>
-    <t>rinc </t>
-  </si>
-  <si>
     <t>right intercostal</t>
   </si>
   <si>
-    <t>linc </t>
-  </si>
-  <si>
     <t>left intercostal</t>
   </si>
   <si>
-    <t>inc </t>
-  </si>
-  <si>
     <t>intercostal</t>
   </si>
   <si>
-    <t>rpv </t>
-  </si>
-  <si>
-    <t>right paravertebral </t>
-  </si>
-  <si>
     <t>left paravertebral</t>
   </si>
   <si>
-    <t>pv </t>
-  </si>
-  <si>
     <t>paravertebral</t>
   </si>
   <si>
-    <t>pa </t>
-  </si>
-  <si>
     <t>paraaortic</t>
   </si>
   <si>
-    <t>rp </t>
-  </si>
-  <si>
     <t>retroperitoneal</t>
   </si>
   <si>
-    <t>um </t>
-  </si>
-  <si>
     <t>upper mediastinal</t>
   </si>
   <si>
     <t>Lower Limb Node Fields</t>
   </si>
   <si>
-    <t>rif </t>
-  </si>
-  <si>
-    <t>right femoral </t>
-  </si>
-  <si>
-    <t>lif </t>
-  </si>
-  <si>
     <t>left femoral</t>
   </si>
   <si>
-    <t>rii </t>
-  </si>
-  <si>
-    <t>right inguinal </t>
-  </si>
-  <si>
-    <t>lii </t>
-  </si>
-  <si>
     <t>left inguinal</t>
   </si>
   <si>
-    <t>riei </t>
-  </si>
-  <si>
-    <t>right external iliac </t>
-  </si>
-  <si>
-    <t>liei </t>
-  </si>
-  <si>
     <t>left external iliac</t>
   </si>
   <si>
-    <t>riii </t>
-  </si>
-  <si>
-    <t>right internal iliac </t>
-  </si>
-  <si>
-    <t>liii </t>
-  </si>
-  <si>
     <t>left internal iliac</t>
   </si>
   <si>
-    <t>rio </t>
-  </si>
-  <si>
-    <t>right obturator </t>
-  </si>
-  <si>
-    <t>lio </t>
-  </si>
-  <si>
     <t>left obturator</t>
   </si>
   <si>
-    <t>ris </t>
-  </si>
-  <si>
-    <t>right pesacral </t>
-  </si>
-  <si>
-    <t>lis </t>
-  </si>
-  <si>
     <t>left pesacral</t>
   </si>
   <si>
-    <t>rpop </t>
-  </si>
-  <si>
-    <t>right popliteal </t>
-  </si>
-  <si>
-    <t>lpop </t>
-  </si>
-  <si>
     <t>left popliteal</t>
   </si>
   <si>
-    <t>in </t>
-  </si>
-  <si>
     <t>interval node</t>
   </si>
   <si>
@@ -444,9 +174,6 @@
     <t>rposta</t>
   </si>
   <si>
-    <t>right postauricular </t>
-  </si>
-  <si>
     <t>Name</t>
   </si>
   <si>
@@ -457,6 +184,288 @@
   </si>
   <si>
     <t>Code</t>
+  </si>
+  <si>
+    <t>ro</t>
+  </si>
+  <si>
+    <t>right occipital</t>
+  </si>
+  <si>
+    <t>rprea</t>
+  </si>
+  <si>
+    <t>right preauricular</t>
+  </si>
+  <si>
+    <t>right postauricular</t>
+  </si>
+  <si>
+    <t>rc1</t>
+  </si>
+  <si>
+    <t>right cervical level i</t>
+  </si>
+  <si>
+    <t>rc2</t>
+  </si>
+  <si>
+    <t>right cervical level ii</t>
+  </si>
+  <si>
+    <t>rc3</t>
+  </si>
+  <si>
+    <t>right cervical level iii</t>
+  </si>
+  <si>
+    <t>rc4</t>
+  </si>
+  <si>
+    <t>right cervical level iv</t>
+  </si>
+  <si>
+    <t>rc5</t>
+  </si>
+  <si>
+    <t>right cervical level v</t>
+  </si>
+  <si>
+    <t>rc6</t>
+  </si>
+  <si>
+    <t>right cervical level vi</t>
+  </si>
+  <si>
+    <t>rc7</t>
+  </si>
+  <si>
+    <t>right cervical level vii</t>
+  </si>
+  <si>
+    <t>rsc</t>
+  </si>
+  <si>
+    <t>right supraclavicular fossa</t>
+  </si>
+  <si>
+    <t>rsm</t>
+  </si>
+  <si>
+    <t>right submental</t>
+  </si>
+  <si>
+    <t>sm</t>
+  </si>
+  <si>
+    <t>rbu</t>
+  </si>
+  <si>
+    <t>right buccal</t>
+  </si>
+  <si>
+    <t>raa</t>
+  </si>
+  <si>
+    <t>ram</t>
+  </si>
+  <si>
+    <t>right mid axilla (levels I,II,III)</t>
+  </si>
+  <si>
+    <t>rap</t>
+  </si>
+  <si>
+    <t>right posterior axilla (levels I,II,III)</t>
+  </si>
+  <si>
+    <t>repit</t>
+  </si>
+  <si>
+    <t>right epitrochlear</t>
+  </si>
+  <si>
+    <t>ric</t>
+  </si>
+  <si>
+    <t>right infraclavicular</t>
+  </si>
+  <si>
+    <t>rtis</t>
+  </si>
+  <si>
+    <t>rip</t>
+  </si>
+  <si>
+    <t>right interpectoral</t>
+  </si>
+  <si>
+    <t>rim</t>
+  </si>
+  <si>
+    <t>right internal mammary</t>
+  </si>
+  <si>
+    <t>rcm</t>
+  </si>
+  <si>
+    <t>right costal margin</t>
+  </si>
+  <si>
+    <t>rinc</t>
+  </si>
+  <si>
+    <t>inc</t>
+  </si>
+  <si>
+    <t>rpv</t>
+  </si>
+  <si>
+    <t>right paravertebral</t>
+  </si>
+  <si>
+    <t>pv</t>
+  </si>
+  <si>
+    <t>pa</t>
+  </si>
+  <si>
+    <t>rp</t>
+  </si>
+  <si>
+    <t>um</t>
+  </si>
+  <si>
+    <t>rif</t>
+  </si>
+  <si>
+    <t>right femoral</t>
+  </si>
+  <si>
+    <t>rii</t>
+  </si>
+  <si>
+    <t>right inguinal</t>
+  </si>
+  <si>
+    <t>riei</t>
+  </si>
+  <si>
+    <t>right external iliac</t>
+  </si>
+  <si>
+    <t>riii</t>
+  </si>
+  <si>
+    <t>right internal iliac</t>
+  </si>
+  <si>
+    <t>rio</t>
+  </si>
+  <si>
+    <t>right obturator</t>
+  </si>
+  <si>
+    <t>ris</t>
+  </si>
+  <si>
+    <t>right pesacral</t>
+  </si>
+  <si>
+    <t>rpop</t>
+  </si>
+  <si>
+    <t>right popliteal</t>
+  </si>
+  <si>
+    <t>in</t>
+  </si>
+  <si>
+    <t>lo</t>
+  </si>
+  <si>
+    <t>lprea</t>
+  </si>
+  <si>
+    <t>lc1</t>
+  </si>
+  <si>
+    <t>lc2</t>
+  </si>
+  <si>
+    <t>lc3</t>
+  </si>
+  <si>
+    <t>lc4</t>
+  </si>
+  <si>
+    <t>lc5</t>
+  </si>
+  <si>
+    <t>lc6</t>
+  </si>
+  <si>
+    <t>lc7</t>
+  </si>
+  <si>
+    <t>lsc</t>
+  </si>
+  <si>
+    <t>lsm</t>
+  </si>
+  <si>
+    <t>lbu</t>
+  </si>
+  <si>
+    <t>laa</t>
+  </si>
+  <si>
+    <t>lam</t>
+  </si>
+  <si>
+    <t>lap</t>
+  </si>
+  <si>
+    <t>lepit</t>
+  </si>
+  <si>
+    <t>lic</t>
+  </si>
+  <si>
+    <t>ltis</t>
+  </si>
+  <si>
+    <t>lip</t>
+  </si>
+  <si>
+    <t>lim</t>
+  </si>
+  <si>
+    <t>lcm</t>
+  </si>
+  <si>
+    <t>linc</t>
+  </si>
+  <si>
+    <t>lif</t>
+  </si>
+  <si>
+    <t>lii</t>
+  </si>
+  <si>
+    <t>liei</t>
+  </si>
+  <si>
+    <t>liii</t>
+  </si>
+  <si>
+    <t>lio</t>
+  </si>
+  <si>
+    <t>lis</t>
+  </si>
+  <si>
+    <t>lpop</t>
   </si>
 </sst>
 </file>
@@ -777,7 +786,7 @@
   <dimension ref="A1:C72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C1" sqref="C1"/>
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -789,21 +798,21 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>143</v>
+        <v>49</v>
       </c>
       <c r="B1" t="s">
-        <v>140</v>
+        <v>46</v>
       </c>
       <c r="C1" t="s">
-        <v>137</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>3</v>
+        <v>50</v>
       </c>
       <c r="B2" t="s">
-        <v>4</v>
+        <v>51</v>
       </c>
       <c r="C2" t="s">
         <v>0</v>
@@ -811,10 +820,10 @@
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B3" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C3" t="s">
         <v>0</v>
@@ -822,10 +831,10 @@
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>138</v>
+        <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>139</v>
+        <v>54</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
@@ -833,10 +842,10 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>55</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>56</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
@@ -844,10 +853,10 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>15</v>
+        <v>57</v>
       </c>
       <c r="B6" t="s">
-        <v>16</v>
+        <v>58</v>
       </c>
       <c r="C6" t="s">
         <v>0</v>
@@ -855,10 +864,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
       <c r="B7" t="s">
-        <v>20</v>
+        <v>60</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
@@ -866,10 +875,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>23</v>
+        <v>61</v>
       </c>
       <c r="B8" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
@@ -877,10 +886,10 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>27</v>
+        <v>63</v>
       </c>
       <c r="B9" t="s">
-        <v>28</v>
+        <v>64</v>
       </c>
       <c r="C9" t="s">
         <v>0</v>
@@ -888,10 +897,10 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>31</v>
+        <v>65</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>66</v>
       </c>
       <c r="C10" t="s">
         <v>0</v>
@@ -899,10 +908,10 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>35</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>68</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
@@ -910,10 +919,10 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>39</v>
+        <v>69</v>
       </c>
       <c r="B12" t="s">
-        <v>40</v>
+        <v>70</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
@@ -921,10 +930,10 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>43</v>
+        <v>71</v>
       </c>
       <c r="B13" t="s">
-        <v>44</v>
+        <v>72</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
@@ -932,10 +941,10 @@
     </row>
     <row r="14" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>47</v>
+        <v>73</v>
       </c>
       <c r="B14" t="s">
-        <v>48</v>
+        <v>14</v>
       </c>
       <c r="C14" t="s">
         <v>0</v>
@@ -943,10 +952,10 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B15" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C15" t="s">
         <v>0</v>
@@ -954,10 +963,10 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>53</v>
+        <v>76</v>
       </c>
       <c r="B16" t="s">
-        <v>54</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>1</v>
@@ -965,10 +974,10 @@
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>57</v>
+        <v>77</v>
       </c>
       <c r="B17" t="s">
-        <v>58</v>
+        <v>78</v>
       </c>
       <c r="C17" t="s">
         <v>1</v>
@@ -976,10 +985,10 @@
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>61</v>
+        <v>79</v>
       </c>
       <c r="B18" t="s">
-        <v>62</v>
+        <v>80</v>
       </c>
       <c r="C18" t="s">
         <v>1</v>
@@ -987,10 +996,10 @@
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>65</v>
+        <v>81</v>
       </c>
       <c r="B19" t="s">
-        <v>66</v>
+        <v>82</v>
       </c>
       <c r="C19" t="s">
         <v>1</v>
@@ -998,10 +1007,10 @@
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>69</v>
+        <v>83</v>
       </c>
       <c r="B20" t="s">
-        <v>70</v>
+        <v>84</v>
       </c>
       <c r="C20" t="s">
         <v>1</v>
@@ -1009,10 +1018,10 @@
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>73</v>
+        <v>85</v>
       </c>
       <c r="B21" t="s">
-        <v>74</v>
+        <v>22</v>
       </c>
       <c r="C21" t="s">
         <v>1</v>
@@ -1020,10 +1029,10 @@
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="B22" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="C22" t="s">
         <v>1</v>
@@ -1031,10 +1040,10 @@
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
-        <v>81</v>
+        <v>88</v>
       </c>
       <c r="B23" t="s">
-        <v>82</v>
+        <v>89</v>
       </c>
       <c r="C23" t="s">
         <v>1</v>
@@ -1042,10 +1051,10 @@
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
-        <v>85</v>
+        <v>90</v>
       </c>
       <c r="B24" t="s">
-        <v>86</v>
+        <v>91</v>
       </c>
       <c r="C24" t="s">
         <v>1</v>
@@ -1053,10 +1062,10 @@
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="B25" t="s">
-        <v>90</v>
+        <v>27</v>
       </c>
       <c r="C25" t="s">
         <v>1</v>
@@ -1067,7 +1076,7 @@
         <v>93</v>
       </c>
       <c r="B26" t="s">
-        <v>94</v>
+        <v>29</v>
       </c>
       <c r="C26" t="s">
         <v>1</v>
@@ -1075,10 +1084,10 @@
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B27" t="s">
         <v>95</v>
-      </c>
-      <c r="B27" t="s">
-        <v>96</v>
       </c>
       <c r="C27" t="s">
         <v>1</v>
@@ -1086,10 +1095,10 @@
     </row>
     <row r="28" spans="1:3" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="B28" t="s">
-        <v>99</v>
+        <v>31</v>
       </c>
       <c r="C28" t="s">
         <v>1</v>
@@ -1097,10 +1106,10 @@
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>100</v>
+        <v>97</v>
       </c>
       <c r="B29" t="s">
-        <v>101</v>
+        <v>32</v>
       </c>
       <c r="C29" t="s">
         <v>1</v>
@@ -1108,10 +1117,10 @@
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="B30" t="s">
-        <v>103</v>
+        <v>33</v>
       </c>
       <c r="C30" t="s">
         <v>1</v>
@@ -1119,10 +1128,10 @@
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>104</v>
+        <v>99</v>
       </c>
       <c r="B31" t="s">
-        <v>105</v>
+        <v>34</v>
       </c>
       <c r="C31" t="s">
         <v>1</v>
@@ -1130,87 +1139,87 @@
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="B32" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="B33" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="C33" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
-        <v>115</v>
+        <v>104</v>
       </c>
       <c r="B34" t="s">
-        <v>116</v>
+        <v>105</v>
       </c>
       <c r="C34" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
       <c r="B35" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
       <c r="C35" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" t="s">
-        <v>123</v>
+        <v>108</v>
       </c>
       <c r="B36" t="s">
-        <v>124</v>
+        <v>109</v>
       </c>
       <c r="C36" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" t="s">
-        <v>127</v>
+        <v>110</v>
       </c>
       <c r="B37" t="s">
-        <v>128</v>
+        <v>111</v>
       </c>
       <c r="C37" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" t="s">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="B38" t="s">
-        <v>132</v>
+        <v>113</v>
       </c>
       <c r="C38" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" t="s">
-        <v>135</v>
+        <v>114</v>
       </c>
       <c r="B39" t="s">
-        <v>136</v>
+        <v>43</v>
       </c>
       <c r="C39" t="s">
         <v>2</v>
@@ -1218,10 +1227,10 @@
     </row>
     <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" t="s">
-        <v>49</v>
+        <v>74</v>
       </c>
       <c r="B40" t="s">
-        <v>50</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
         <v>2</v>
@@ -1229,10 +1238,10 @@
     </row>
     <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" t="s">
-        <v>5</v>
+        <v>115</v>
       </c>
       <c r="B41" t="s">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="C41" t="s">
         <v>0</v>
@@ -1240,10 +1249,10 @@
     </row>
     <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" t="s">
-        <v>9</v>
+        <v>116</v>
       </c>
       <c r="B42" t="s">
-        <v>10</v>
+        <v>4</v>
       </c>
       <c r="C42" t="s">
         <v>0</v>
@@ -1251,10 +1260,10 @@
     </row>
     <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" t="s">
-        <v>141</v>
+        <v>47</v>
       </c>
       <c r="B43" t="s">
-        <v>142</v>
+        <v>48</v>
       </c>
       <c r="C43" t="s">
         <v>0</v>
@@ -1262,10 +1271,10 @@
     </row>
     <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" t="s">
-        <v>13</v>
+        <v>117</v>
       </c>
       <c r="B44" t="s">
-        <v>14</v>
+        <v>5</v>
       </c>
       <c r="C44" t="s">
         <v>0</v>
@@ -1273,10 +1282,10 @@
     </row>
     <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" t="s">
-        <v>17</v>
+        <v>118</v>
       </c>
       <c r="B45" t="s">
-        <v>18</v>
+        <v>6</v>
       </c>
       <c r="C45" t="s">
         <v>0</v>
@@ -1284,10 +1293,10 @@
     </row>
     <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" t="s">
-        <v>21</v>
+        <v>119</v>
       </c>
       <c r="B46" t="s">
-        <v>22</v>
+        <v>7</v>
       </c>
       <c r="C46" t="s">
         <v>0</v>
@@ -1295,10 +1304,10 @@
     </row>
     <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" t="s">
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="B47" t="s">
-        <v>26</v>
+        <v>8</v>
       </c>
       <c r="C47" t="s">
         <v>0</v>
@@ -1306,10 +1315,10 @@
     </row>
     <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" t="s">
-        <v>29</v>
+        <v>121</v>
       </c>
       <c r="B48" t="s">
-        <v>30</v>
+        <v>9</v>
       </c>
       <c r="C48" t="s">
         <v>0</v>
@@ -1317,10 +1326,10 @@
     </row>
     <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" t="s">
-        <v>33</v>
+        <v>122</v>
       </c>
       <c r="B49" t="s">
-        <v>34</v>
+        <v>10</v>
       </c>
       <c r="C49" t="s">
         <v>0</v>
@@ -1328,10 +1337,10 @@
     </row>
     <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" t="s">
-        <v>37</v>
+        <v>123</v>
       </c>
       <c r="B50" t="s">
-        <v>38</v>
+        <v>11</v>
       </c>
       <c r="C50" t="s">
         <v>0</v>
@@ -1339,10 +1348,10 @@
     </row>
     <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" t="s">
-        <v>41</v>
+        <v>124</v>
       </c>
       <c r="B51" t="s">
-        <v>42</v>
+        <v>12</v>
       </c>
       <c r="C51" t="s">
         <v>0</v>
@@ -1350,10 +1359,10 @@
     </row>
     <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" t="s">
-        <v>45</v>
+        <v>125</v>
       </c>
       <c r="B52" t="s">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="C52" t="s">
         <v>0</v>
@@ -1361,10 +1370,10 @@
     </row>
     <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C53" t="s">
         <v>0</v>
@@ -1372,10 +1381,10 @@
     </row>
     <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="B54" t="s">
-        <v>56</v>
+        <v>17</v>
       </c>
       <c r="C54" t="s">
         <v>1</v>
@@ -1383,10 +1392,10 @@
     </row>
     <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" t="s">
-        <v>59</v>
+        <v>128</v>
       </c>
       <c r="B55" t="s">
-        <v>60</v>
+        <v>18</v>
       </c>
       <c r="C55" t="s">
         <v>1</v>
@@ -1394,10 +1403,10 @@
     </row>
     <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" t="s">
-        <v>63</v>
+        <v>129</v>
       </c>
       <c r="B56" t="s">
-        <v>64</v>
+        <v>19</v>
       </c>
       <c r="C56" t="s">
         <v>1</v>
@@ -1405,10 +1414,10 @@
     </row>
     <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" t="s">
-        <v>67</v>
+        <v>130</v>
       </c>
       <c r="B57" t="s">
-        <v>68</v>
+        <v>20</v>
       </c>
       <c r="C57" t="s">
         <v>1</v>
@@ -1416,10 +1425,10 @@
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
-        <v>71</v>
+        <v>131</v>
       </c>
       <c r="B58" t="s">
-        <v>72</v>
+        <v>21</v>
       </c>
       <c r="C58" t="s">
         <v>1</v>
@@ -1427,10 +1436,10 @@
     </row>
     <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
-        <v>75</v>
+        <v>132</v>
       </c>
       <c r="B59" t="s">
-        <v>76</v>
+        <v>23</v>
       </c>
       <c r="C59" t="s">
         <v>1</v>
@@ -1438,10 +1447,10 @@
     </row>
     <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" t="s">
-        <v>79</v>
+        <v>133</v>
       </c>
       <c r="B60" t="s">
-        <v>80</v>
+        <v>24</v>
       </c>
       <c r="C60" t="s">
         <v>1</v>
@@ -1449,10 +1458,10 @@
     </row>
     <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" t="s">
-        <v>83</v>
+        <v>134</v>
       </c>
       <c r="B61" t="s">
-        <v>84</v>
+        <v>25</v>
       </c>
       <c r="C61" t="s">
         <v>1</v>
@@ -1460,10 +1469,10 @@
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" t="s">
-        <v>87</v>
+        <v>135</v>
       </c>
       <c r="B62" t="s">
-        <v>88</v>
+        <v>26</v>
       </c>
       <c r="C62" t="s">
         <v>1</v>
@@ -1471,10 +1480,10 @@
     </row>
     <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" t="s">
-        <v>91</v>
+        <v>136</v>
       </c>
       <c r="B63" t="s">
-        <v>92</v>
+        <v>28</v>
       </c>
       <c r="C63" t="s">
         <v>1</v>
@@ -1482,10 +1491,10 @@
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B64" t="s">
-        <v>97</v>
+        <v>30</v>
       </c>
       <c r="C64" t="s">
         <v>1</v>
@@ -1493,87 +1502,87 @@
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" t="s">
-        <v>109</v>
+        <v>137</v>
       </c>
       <c r="B65" t="s">
-        <v>110</v>
+        <v>36</v>
       </c>
       <c r="C65" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" t="s">
-        <v>113</v>
+        <v>138</v>
       </c>
       <c r="B66" t="s">
-        <v>114</v>
+        <v>37</v>
       </c>
       <c r="C66" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" t="s">
-        <v>117</v>
+        <v>139</v>
       </c>
       <c r="B67" t="s">
-        <v>118</v>
+        <v>38</v>
       </c>
       <c r="C67" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" t="s">
-        <v>121</v>
+        <v>140</v>
       </c>
       <c r="B68" t="s">
-        <v>122</v>
+        <v>39</v>
       </c>
       <c r="C68" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" t="s">
-        <v>125</v>
+        <v>141</v>
       </c>
       <c r="B69" t="s">
-        <v>126</v>
+        <v>40</v>
       </c>
       <c r="C69" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" t="s">
-        <v>129</v>
+        <v>142</v>
       </c>
       <c r="B70" t="s">
-        <v>130</v>
+        <v>41</v>
       </c>
       <c r="C70" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" t="s">
-        <v>133</v>
+        <v>143</v>
       </c>
       <c r="B71" t="s">
-        <v>134</v>
+        <v>42</v>
       </c>
       <c r="C71" t="s">
-        <v>106</v>
+        <v>35</v>
       </c>
     </row>
     <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" t="s">
-        <v>51</v>
+        <v>126</v>
       </c>
       <c r="B72" t="s">
-        <v>52</v>
+        <v>15</v>
       </c>
       <c r="C72" t="s">
         <v>2</v>

</xml_diff>